<commit_message>
version 2 text changes, payment html and function updated , eeg button changes, register bootstrap popover and consent text
</commit_message>
<xml_diff>
--- a/app/static/csv/about_app.xlsx
+++ b/app/static/csv/about_app.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\ruchella\agestudy\app\static\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{9812C7D8-2E85-402B-9706-89EF2B367824}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE09757B-428C-49B8-9DCF-CEAC1250E95D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2640" windowWidth="14400" windowHeight="7590"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="about_app" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="138">
   <si>
     <t>tag</t>
   </si>
@@ -40,27 +40,12 @@
     <t>Waar kan ik de app downloaden?  Is de app gratis?</t>
   </si>
   <si>
-    <t>p1</t>
-  </si>
-  <si>
-    <t>Ja de app is gratis! U kunt de app downloaden via </t>
-  </si>
-  <si>
-    <t>Yes! It is free and you can download it at</t>
-  </si>
-  <si>
     <t>h12</t>
   </si>
   <si>
-    <t>I just signed up on Agestudy.nl and installed the App, what should I do next?</t>
-  </si>
-  <si>
     <t>p2</t>
   </si>
   <si>
-    <t>You will receive an email within the coming days with further instructions, including your participation ID which needs to be pasted into the App.</t>
-  </si>
-  <si>
     <t>h13</t>
   </si>
   <si>
@@ -73,12 +58,6 @@
     <t>Yes, this is normal and may remain like this for the next few hours. If it persists for more than a day then please email us at agestudy@leidenuniv.nl</t>
   </si>
   <si>
-    <t xml:space="preserve">Ik heb me net aangemeld op Agestudy.nl en de app geïnstalleerd, wat moet ik nu doen? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">U ontvangt de komende dagen een e-mail met verdere instructies, inclusief uw deelname-ID. Uw deelname-ID moet in de app worden geplakt. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Na installatie van de app zegt mijn app ‘Calibrating’ is dit normaal? </t>
   </si>
   <si>
@@ -88,9 +67,6 @@
     <t>h14</t>
   </si>
   <si>
-    <t>Ik heb zojuist een e-mail ontvangen met mijn deelname-ID, wat moet ik hiermee doen?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Plak deze ID in elke Android-smartphonetablet die alleen door u gebruikt wordt. </t>
   </si>
   <si>
@@ -115,9 +91,6 @@
     <t xml:space="preserve">Stap 3. In ‘participate’ kunt u de ID plakken. Volg de gele vlekken om te plakken. </t>
   </si>
   <si>
-    <t>I just got an email with my participation ID, what should I do with it?</t>
-  </si>
-  <si>
     <t>Please paste this ID into any Android smartphone tablet that you (alone) use</t>
   </si>
   <si>
@@ -172,18 +145,12 @@
     <t>Follow the yellow spots after launching the TapCounter App, but remember to be on WiFi or 3G or 4G internet while doing so.</t>
   </si>
   <si>
-    <t xml:space="preserve">Ik heb zojuist een e-mail ontvangen met het verzoek om een 'handmatige synchronisatie', hoe kan ik dat doen? </t>
-  </si>
-  <si>
     <t xml:space="preserve">Volg de gele vlekken na het starten van de TapCounter-app,  vergeet hierbij niet de telefoon te verbinden met WiFi, 3G of 4G (internet). </t>
   </si>
   <si>
     <t>h18</t>
   </si>
   <si>
-    <t xml:space="preserve">Ik heb zojuist een e-mail ontvangen met mijn APP-ID, hoe stuur ik het naar u op? </t>
-  </si>
-  <si>
     <t xml:space="preserve">Kopieer uw APP-ID van ELKE Android-smartphone en -tablet die u (als enige) gebruikt. </t>
   </si>
   <si>
@@ -196,9 +163,6 @@
     <t>p8</t>
   </si>
   <si>
-    <t>I just got an email requesting my APP ID, what is it and how do I send it to you?</t>
-  </si>
-  <si>
     <t>Please copy your APP ID from every Android smartphone and tablet that you (and no one else) use.</t>
   </si>
   <si>
@@ -217,9 +181,6 @@
     <t>h19</t>
   </si>
   <si>
-    <t>I just got an email requesting I re-instate the ‘Apps that can appear on top’ permissions, what do I do?</t>
-  </si>
-  <si>
     <t>p9</t>
   </si>
   <si>
@@ -238,12 +199,6 @@
     <t>The ’Apps that can appear on top’ setting may be called differently, for example ’Display over other apps’.</t>
   </si>
   <si>
-    <t xml:space="preserve">Ik heb zojuist een e-mail ontvangen met het verzoek de ‘Apps die bovenaan kunnen worden weergegeven’ opnieuw in te stellen, wat moet ik doen? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">De eenvoudigste manier is om te zoeken naar 'Bovenaan verschijnen' of 'Weergeven vóór andere apps' in het zoekveld van de instellingen. Klik hierop en blader naar TapCounter en stel het in. Zie de onderstaande stappen: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Als dit niet werkt, kunt u het als volgt proberen: </t>
   </si>
   <si>
@@ -262,15 +217,9 @@
     <t>Again, the ‘Usage data setting‘ may be called differently, for example ’Apps with usage access’.</t>
   </si>
   <si>
-    <t xml:space="preserve">Ik heb zojuist een e-mail ontvangen met het verzoek de rechten voor ‘Gebruikstoegang’ opnieuw in te stellen, wat moet ik doen? </t>
-  </si>
-  <si>
     <t xml:space="preserve">Nogmaals, de ‘Gebruiksgegevensinstelling’ kan anders worden genoemd, bijvoorbeeld ‘Apps met gebruikstoegang’. </t>
   </si>
   <si>
-    <t>I just got an email requesting a ‘manual sync’, how do I do that?</t>
-  </si>
-  <si>
     <t>p13</t>
   </si>
   <si>
@@ -281,9 +230,6 @@
   </si>
   <si>
     <t>What data is collected by the TapCounter App?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">De eenvoudigste manier is om in het zoekveld van de instellingen ‘gebruikstoegang tot gegevens’ of ‘gebruikstoegang’ te zoeken. Klik daarop en blader naar TapCounter en stel het in. Zie de onderstaande stappen: </t>
   </si>
   <si>
     <t>li_data_app_1</t>
@@ -397,8 +343,87 @@
     </r>
   </si>
   <si>
+    <t>Het onderzoeksteam van de Universiteit Leiden gebruikt deze app voor dit onderzoek. Deze app wordt beheerd door de University of Zurich Spin-off QuantActions Ltd (Lausanne, Zwitserland) en u kunt het gedetailleerde privacybeleid hier vinden. Google PlayStore wordt gebruikt om deze app te distribueren naar gebruikers zoals u. </t>
+  </si>
+  <si>
+    <t>h24</t>
+  </si>
+  <si>
+    <t>p17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">De app is ontworpen om de gegevens bij voorkeur met WiFI te synchroniseren,  
+na meerdere mislukte pogingen zal deze gebruikmaken van 3G- of 4G-internet. 
+De datasynchronisaties zijn echter klein, variërend van enkele KB tot enkele MB per maand. 
+Dat wil zeggen, zo klein als bijvoorbeeld een enkele foto vastgelegd met een smartphone per maand. </t>
+  </si>
+  <si>
+    <t>Hoe zorg ik ervoor dat de app operationeel blijft?</t>
+  </si>
+  <si>
+    <t>I just signed up on www.Agestudy.nl and installed the App, what should I do next?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ik heb me net aangemeld op www.Agestudy.nl en de app geïnstalleerd, wat moet ik nu doen? </t>
+  </si>
+  <si>
+    <t>pp1</t>
+  </si>
+  <si>
+    <t>pp2</t>
+  </si>
+  <si>
+    <t>pp3</t>
+  </si>
+  <si>
+    <t>Yes it is free!</t>
+  </si>
+  <si>
+    <t>pp0</t>
+  </si>
+  <si>
+    <t>Ja de app is gratis!</t>
+  </si>
+  <si>
+    <t>U kunt de App eenvoudig stoppen door hem te verwijderen. Let op, om u formeel terug te trekken uit het onderzoek, stuur ons alstublieft een mail. Om te verwijderen, druk lang op het App-icoon en klik op 'Verwijderen'.</t>
+  </si>
+  <si>
     <r>
-      <t>Wie is de organisaties achter de TapCounter-app?</t>
+      <t>Download and open the app</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Download en open de app</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>You will receive an email from Leiden University within the coming days with further instructions, including your participation ID which needs to be pasted into the App.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U ontvangt de komende dagen een e-mail van de Universiteit Leiden met verdere instructies, inclusief uw deelname-ID. Uw deelname-ID moet in de app worden geplakt. </t>
+  </si>
+  <si>
+    <r>
+      <t>Wat is de organisatie achter de TapCounter app?</t>
     </r>
     <r>
       <rPr>
@@ -412,29 +437,114 @@
     </r>
   </si>
   <si>
-    <t>Het onderzoeksteam van de Universiteit Leiden gebruikt deze app voor dit onderzoek. Deze app wordt beheerd door de University of Zurich Spin-off QuantActions Ltd (Lausanne, Zwitserland) en u kunt het gedetailleerde privacybeleid hier vinden. Google PlayStore wordt gebruikt om deze app te distribueren naar gebruikers zoals u. </t>
-  </si>
-  <si>
-    <t>h24</t>
-  </si>
-  <si>
-    <t>p17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">De app is ontworpen om de gegevens bij voorkeur met WiFI te synchroniseren,  
-na meerdere mislukte pogingen zal deze gebruikmaken van 3G- of 4G-internet. 
-De datasynchronisaties zijn echter klein, variërend van enkele KB tot enkele MB per maand. 
-Dat wil zeggen, zo klein als bijvoorbeeld een enkele foto vastgelegd met een smartphone per maand. </t>
-  </si>
-  <si>
-    <t>I just got an email requesting I re-instate the ‘Usage access’ permissions, what do I do?</t>
+    <t>Ik heb zojuist een e-mail ontvangen van de Universiteit Leiden met het verzoek de ‘Apps die bovenop kunnen worden weergegeven’ opnieuw in te stellen, wat moet ik doen?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">De eenvoudigste manier is om te zoeken naar ‘Bovenop weergeven’ in het zoekveld van de instellingen. Klik hierop en blader naar TapCounter en stel het in. Zie de onderstaande stappen: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ik heb zojuist een e-mail ontvangen van de Universiteit Leiden met het verzoek de rechten voor ‘Toegang gebruiksgegevens’ opnieuw in te stellen, wat moet ik doen? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">De eenvoudigste manier is om in het zoekveld van de instellingen ‘Toegang gebruiksgegevens’ te zoeken. Klik daarop en blader naar TapCounter en stel het in. Zie de onderstaande stappen: </t>
+  </si>
+  <si>
+    <t>Ik heb zojuist een e-mail ontvangen van de Universiteit Leiden met mijn deelname-ID, wat moet ik hiermee doen?</t>
+  </si>
+  <si>
+    <t>I just got an email from Leiden University with my participation ID, what should I do with it?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ik heb zojuist een e-mail ontvangen van de Universiteit Leiden met het verzoek om een ‘handmatige synchronisatie’, hoe kan ik dat doen? </t>
+  </si>
+  <si>
+    <t>I just got an email from Leiden University requesting a ‘manual sync’, how do I do that?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ik heb zojuist een e-mail ontvangen van de Universiteit Leiden met mijn APP-ID, hoe stuur ik het naar u op? </t>
+  </si>
+  <si>
+    <t>I just got an email from Leiden University requesting my APP ID, what is it and how do I send it to you?</t>
+  </si>
+  <si>
+    <t>I just got an email from Leiden University requesting I re-instate the ‘Apps that can appear on top’ permissions, what do I do?</t>
+  </si>
+  <si>
+    <t>I just got an email from Leiden University requesting I re-instate the ‘Usage access’ permissions, what do I do?</t>
+  </si>
+  <si>
+    <r>
+      <t>Type “QuantActions TapCounter” in de zoekbalk. &lt;b&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF212529"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Voer het precies zo in.&lt;/b&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF212529"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> Zorg ervoor dat u de app downloadt van de maker genaamd Quant{Actions} OF klik &lt;a target=_blank_  href="https://play.google.com/store/apps/details?id=com.quantactions.tapcounter"&gt;HIER&lt;/a&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Type “QuantActions TapCounter” in the search bar. &lt;b&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF212529"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Put it exactly like that.&lt;/b&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF212529"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> Make sure you are downloading the app from the creator called Quant{Actions}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> OR click &lt;a target=_blank_  href="https://play.google.com/store/apps/details?id=com.quantactions.tapcounter"&gt;HERE&lt;/a&gt;. </t>
+    </r>
+  </si>
+  <si>
+    <t>Ga naar de &lt;a target=_blank_  href="https://play.google.com/store/"&gt;Google Play Store&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Go to the &lt;a target=_blank_  href="https://play.google.com/store/"&gt;Google Play Store&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="21" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -586,6 +696,27 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF212529"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF212529"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -932,13 +1063,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1294,11 +1428,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B15" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1330,463 +1464,743 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>114</v>
+      </c>
+      <c r="B3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
+        <v>111</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>39</v>
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>82</v>
+        <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>59</v>
+        <v>129</v>
       </c>
       <c r="C20" t="s">
-        <v>54</v>
+        <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>55</v>
+        <v>40</v>
+      </c>
+      <c r="C21" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>61</v>
+        <v>131</v>
       </c>
       <c r="C22" t="s">
-        <v>56</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C24" t="s">
-        <v>73</v>
+        <v>48</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>71</v>
+        <v>132</v>
       </c>
       <c r="C26" t="s">
-        <v>75</v>
+        <v>122</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>126</v>
+        <v>54</v>
       </c>
       <c r="C27" t="s">
-        <v>80</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="C28" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C29" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>79</v>
+        <v>133</v>
       </c>
       <c r="C30" t="s">
-        <v>81</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="C31" t="s">
-        <v>95</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>96</v>
+        <v>55</v>
+      </c>
+      <c r="C32" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>104</v>
+        <v>64</v>
       </c>
       <c r="C33" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>105</v>
+        <v>69</v>
       </c>
       <c r="C34" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>100</v>
+        <v>86</v>
+      </c>
+      <c r="C36" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>101</v>
+        <v>87</v>
+      </c>
+      <c r="C37" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>110</v>
+        <v>74</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="60.75" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>112</v>
+        <v>75</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>125</v>
+        <v>90</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>114</v>
+        <v>76</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>121</v>
+        <v>91</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>123</v>
+        <v>94</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>118</v>
+        <v>95</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>119</v>
+        <v>97</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>98</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>104</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C46" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>105</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007D896C3867AA3F4EB0C0DE718E7AD517" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="80024e68534539ed8e026f0b5c1f9e6f">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c478e2cf-1bd2-4bab-9bac-f508c15c8b21" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3dc892a718835b0a8dea2591f8ec0eaf" ns3:_="">
+    <xsd:import namespace="c478e2cf-1bd2-4bab-9bac-f508c15c8b21"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="c478e2cf-1bd2-4bab-9bac-f508c15c8b21" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoTags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="11" nillable="true" ma:displayName="MediaServiceOCR" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="12" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="13" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="14" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="15" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="16" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EA2A4B5-4A93-4099-B978-EB4B70751D3B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03D7A8B8-DE8F-4F05-BCF1-D0405792B2DC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="c478e2cf-1bd2-4bab-9bac-f508c15c8b21"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3331CACC-F63C-4322-882B-00BE6F100C27}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="c478e2cf-1bd2-4bab-9bac-f508c15c8b21"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
checkbox on home and test page, recaptha, share button, psytoolkit link with unique id, text updates and images updates
</commit_message>
<xml_diff>
--- a/app/static/csv/about_app.xlsx
+++ b/app/static/csv/about_app.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\ruchella\agestudy\app\static\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE09757B-428C-49B8-9DCF-CEAC1250E95D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B9EB07F-046D-466B-B692-EBCDB0D53CD4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="about_app" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="139">
   <si>
     <t>tag</t>
   </si>
@@ -52,18 +52,6 @@
     <t>p3</t>
   </si>
   <si>
-    <t>After installation, my App says it is ‘Calibrating’ is this normal?</t>
-  </si>
-  <si>
-    <t>Yes, this is normal and may remain like this for the next few hours. If it persists for more than a day then please email us at agestudy@leidenuniv.nl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Na installatie van de app zegt mijn app ‘Calibrating’ is dit normaal? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ja, dit is normaal dit kan de komende uren zo blijven. Als het langer dan een dag duurt, stuur ons dan een e-mail op agestudy@leidenuniv.nl </t>
-  </si>
-  <si>
     <t>h14</t>
   </si>
   <si>
@@ -202,9 +190,6 @@
     <t xml:space="preserve">Als dit niet werkt, kunt u het als volgt proberen: </t>
   </si>
   <si>
-    <t xml:space="preserve">De ‘Apps die bovenaan kunnen verschijnen’ kunnen anders worden genoemd, bijvoorbeeld ‘Weergeven vóór andere apps’. </t>
-  </si>
-  <si>
     <t>h20</t>
   </si>
   <si>
@@ -214,18 +199,9 @@
     <t>The simplest way may be to search ‘usage data access’ or ‘apps with usage access’ into the search field of the settings. Click on that and then scroll to TapCounter and tun it on. See the steps below:</t>
   </si>
   <si>
-    <t>Again, the ‘Usage data setting‘ may be called differently, for example ’Apps with usage access’.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nogmaals, de ‘Gebruiksgegevensinstelling’ kan anders worden genoemd, bijvoorbeeld ‘Apps met gebruikstoegang’. </t>
-  </si>
-  <si>
     <t>p13</t>
   </si>
   <si>
-    <t>p14</t>
-  </si>
-  <si>
     <t>h21</t>
   </si>
   <si>
@@ -254,48 +230,6 @@
   </si>
   <si>
     <t xml:space="preserve">Welke gegevens worden verzameld door de TapCounter-app? </t>
-  </si>
-  <si>
-    <t>De unieke identificatie die willekeurig door de app wordt gegenereerd, zoals: 138xxxiwhhwhh992ef. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fabrikant en model van de smartphone zoals: SAMSUNG A10. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Versienummer van het Android-besturingssysteem zoals:  versie 10.0. </t>
-  </si>
-  <si>
-    <t>Ruwe locatie zoals: Leiden, Nederland (informatie over positie met 0 decimalen). </t>
-  </si>
-  <si>
-    <t>Het tijdstempel van de touchscreen-aanraking zoals: 20 januari 2020, 10u, 5m, 10s, 5ms. </t>
-  </si>
-  <si>
-    <t>Het label van de app die gebruik wordt zoals:  Facebook of Weer. </t>
-  </si>
-  <si>
-    <t>Of uw telefoon in de staande of liggende modus werd gebruikt. </t>
-  </si>
-  <si>
-    <t>The unique identifier randomly generated by the App as in 138xxxiwhhwhh992ef.</t>
-  </si>
-  <si>
-    <t>Manufacturer and model of the smartphone as in SAMSUNG A10.</t>
-  </si>
-  <si>
-    <t>Android operating system version number as in version 10.0.</t>
-  </si>
-  <si>
-    <t>Rough location as in Leiden, Netherlands (0 decimal position information).</t>
-  </si>
-  <si>
-    <t>The timestamp of the touchscreen touch as in 20th Jan 2020, 10h,5m,10s,5ms.</t>
-  </si>
-  <si>
-    <t>The label of the App in use as in Facebook or Weather.</t>
-  </si>
-  <si>
-    <t>If your phone was used in the portrait or landscape mode.</t>
   </si>
   <si>
     <t>h22</t>
@@ -358,9 +292,6 @@
 Dat wil zeggen, zo klein als bijvoorbeeld een enkele foto vastgelegd met een smartphone per maand. </t>
   </si>
   <si>
-    <t>Hoe zorg ik ervoor dat de app operationeel blijft?</t>
-  </si>
-  <si>
     <t>I just signed up on www.Agestudy.nl and installed the App, what should I do next?</t>
   </si>
   <si>
@@ -383,9 +314,6 @@
   </si>
   <si>
     <t>Ja de app is gratis!</t>
-  </si>
-  <si>
-    <t>U kunt de App eenvoudig stoppen door hem te verwijderen. Let op, om u formeel terug te trekken uit het onderzoek, stuur ons alstublieft een mail. Om te verwijderen, druk lang op het App-icoon en klik op 'Verwijderen'.</t>
   </si>
   <si>
     <r>
@@ -538,6 +466,81 @@
   </si>
   <si>
     <t>Go to the &lt;a target=_blank_  href="https://play.google.com/store/"&gt;Google Play Store&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>p8a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Om de APP-ID te sturen, open uw e-mail app (bv. Gmail), maak een nieuw bericht naar agestudy@fsw.leidenuniv.nl en druk met uw vinger op het scherm totdat de ‘Plakken’ optie verschijnt. Als u dan op ‘Plakken’ drukt, zal de APP-ID als tekst verschijnen. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">To send the ID via e-mail, open your e-mail app (e.g. Gmail), create a new concept to agestudy@fsw.leidenuniv.nl and press the blank e-mail space with your finger until the ‘Paste’ option appears. When you click on ‘Paste’, the ID should show as text in that space. </t>
+  </si>
+  <si>
+    <t>De instelling optie ‘Weergeven vóór andere apps’ kan een ander naam hebben in uw telefoon, bijvoorbeeld ‘Bovenaan verschijnen’ of ‘Over andere apps tekenen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hoe kan ik de App stoppen met het meten van mijn gegevens? </t>
+  </si>
+  <si>
+    <t>U kunt de App stoppen door deze gewoon te verwijderen. Let op, stuur ons alstublieft een mail om u formeel terug te trekken uit het onderzoek. Om de App te verwijderen, druk lang op het App-icoon en klik op 'Verwijderen'.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start de App eens in de 2-3 dagen. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ja, dit is normaal dit kan de komende uren zo blijven. Als het langer dan een dag duurt, stuur ons dan een e-mail op agestudy@fsw.leidenuniv.nl </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Na installatie van de app zegt mijn app ‘Initialising’ is dit normaal? </t>
+  </si>
+  <si>
+    <t>After installation, my App says it is ‘Initialising’ is this normal?</t>
+  </si>
+  <si>
+    <t>Yes, this is normal and may remain like this for the next few hours. If it persists for more than a day then please email us at agestudy@fsw.leidenuniv.nl</t>
+  </si>
+  <si>
+    <t>The unique identifier randomly generated by the App as in 138xxxiwhhwhh992ef</t>
+  </si>
+  <si>
+    <t>Manufacturer and model of the smartphone as in SAMSUNG A10</t>
+  </si>
+  <si>
+    <t>Android operating system version number as in version 10.0</t>
+  </si>
+  <si>
+    <t>Rough location as in Leiden, Netherlands (0 decimal position information)</t>
+  </si>
+  <si>
+    <t>The timestamp of the touchscreen touch as in 20th Jan 2020, 10h,5m,10s,5ms</t>
+  </si>
+  <si>
+    <t>The label of the App in use as in Facebook or Weather</t>
+  </si>
+  <si>
+    <t>If your phone was used in the portrait or landscape mode</t>
+  </si>
+  <si>
+    <t>Het tijdstempel van de touchscreen-aanraking zoals: 20 januari 2020, 10u, 5m, 10s, 5ms</t>
+  </si>
+  <si>
+    <t>Ruwe locatie zoals: Leiden, Nederland (informatie over positie met 0 decimalen)</t>
+  </si>
+  <si>
+    <t>Versienummer van het Android-besturingssysteem zoals:  versie 10.0</t>
+  </si>
+  <si>
+    <t>Fabrikant en model van de smartphone zoals: SAMSUNG A10</t>
+  </si>
+  <si>
+    <t>De unieke identificatie die willekeurig door de app wordt gegenereerd, zoals: 138xxxiwhhwhh992ef</t>
+  </si>
+  <si>
+    <t>Het label van de app die gebruik wordt zoals:  Facebook of Weer</t>
+  </si>
+  <si>
+    <t>Of uw telefoon in de staande of liggende modus werd gebruikt</t>
   </si>
 </sst>
 </file>
@@ -1431,18 +1434,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="C28" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="220" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="255.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1453,7 +1456,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1464,504 +1467,504 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="B3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="C3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C4" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="C7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="C8" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>123</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
         <v>11</v>
       </c>
-      <c r="C10" t="s">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C20" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
+        <v>114</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+      <c r="A27" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C27" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+      <c r="A28" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+      <c r="A29" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+      <c r="A30" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+      <c r="A31" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C31" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+      <c r="A32" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+      <c r="A33" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+      <c r="A34" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+      <c r="A35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+      <c r="A36" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C36" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+      <c r="A37" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C11" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="2" t="s">
+      <c r="C37" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+      <c r="A38" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+      <c r="A39" t="s">
+        <v>66</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C20" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="2" t="s">
+      <c r="C39" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+      <c r="A40" t="s">
+        <v>67</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+      <c r="A41" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C22" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>46</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>51</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>52</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C26" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>53</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>56</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>57</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>61</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C30" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>62</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C31" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>66</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C32" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>67</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C33" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>68</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="C41" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+      <c r="A42" t="s">
+        <v>70</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="58.5" x14ac:dyDescent="0.4">
+      <c r="A43" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+      <c r="A44" t="s">
+        <v>74</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+      <c r="A45" t="s">
+        <v>76</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>70</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C35" s="1" t="s">
+      <c r="C45" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+      <c r="A46" t="s">
+        <v>82</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>71</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="C46" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+      <c r="A47" t="s">
+        <v>83</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>72</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C37" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>73</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>74</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>75</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>76</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>92</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="60.75" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>94</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>96</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>98</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>104</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C46" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>105</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="C47" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C48" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1971,15 +1974,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007D896C3867AA3F4EB0C0DE718E7AD517" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="80024e68534539ed8e026f0b5c1f9e6f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c478e2cf-1bd2-4bab-9bac-f508c15c8b21" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3dc892a718835b0a8dea2591f8ec0eaf" ns3:_="">
     <xsd:import namespace="c478e2cf-1bd2-4bab-9bac-f508c15c8b21"/>
@@ -2157,6 +2151,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2164,14 +2167,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EA2A4B5-4A93-4099-B978-EB4B70751D3B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03D7A8B8-DE8F-4F05-BCF1-D0405792B2DC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2185,6 +2180,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EA2A4B5-4A93-4099-B978-EB4B70751D3B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
CRT added, automatic email, password reset, navbar language from dropdown to button, small textual changes
</commit_message>
<xml_diff>
--- a/app/static/csv/about_app.xlsx
+++ b/app/static/csv/about_app.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\ruchella\agestudy\app\static\csv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fswleidenunivnl-my.sharepoint.com/personal/a_ghosh_fsw_leidenuniv_nl/Documents/Leiden_CODELAB/Velux_Age/LabSetUp/OnlineTests/Web_based_testing/Online Texts/csvtranslate_v2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B9EB07F-046D-466B-B692-EBCDB0D53CD4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{64033121-2941-41AB-BF0E-307FC7950404}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="about_app" sheetId="1" r:id="rId1"/>
@@ -290,12 +290,6 @@
 na meerdere mislukte pogingen zal deze gebruikmaken van 3G- of 4G-internet. 
 De datasynchronisaties zijn echter klein, variërend van enkele KB tot enkele MB per maand. 
 Dat wil zeggen, zo klein als bijvoorbeeld een enkele foto vastgelegd met een smartphone per maand. </t>
-  </si>
-  <si>
-    <t>I just signed up on www.Agestudy.nl and installed the App, what should I do next?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ik heb me net aangemeld op www.Agestudy.nl en de app geïnstalleerd, wat moet ik nu doen? </t>
   </si>
   <si>
     <t>pp1</t>
@@ -474,9 +468,6 @@
     <t xml:space="preserve">Om de APP-ID te sturen, open uw e-mail app (bv. Gmail), maak een nieuw bericht naar agestudy@fsw.leidenuniv.nl en druk met uw vinger op het scherm totdat de ‘Plakken’ optie verschijnt. Als u dan op ‘Plakken’ drukt, zal de APP-ID als tekst verschijnen. </t>
   </si>
   <si>
-    <t xml:space="preserve">To send the ID via e-mail, open your e-mail app (e.g. Gmail), create a new concept to agestudy@fsw.leidenuniv.nl and press the blank e-mail space with your finger until the ‘Paste’ option appears. When you click on ‘Paste’, the ID should show as text in that space. </t>
-  </si>
-  <si>
     <t>De instelling optie ‘Weergeven vóór andere apps’ kan een ander naam hebben in uw telefoon, bijvoorbeeld ‘Bovenaan verschijnen’ of ‘Over andere apps tekenen</t>
   </si>
   <si>
@@ -541,6 +532,15 @@
   </si>
   <si>
     <t>Of uw telefoon in de staande of liggende modus werd gebruikt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To send the ID via e-mail, open your e-mail app (e.g. Gmail), create a new email to agestudy@fsw.leidenuniv.nl and press the blank e-mail space with your finger until the ‘Paste’ option appears. When you click on ‘Paste’, the ID should show as text in that space. </t>
+  </si>
+  <si>
+    <t>I just signed up on Agestudy.nl and installed the App, what should I do next?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ik heb me net aangemeld op Agestudy.nl en de app geïnstalleerd, wat moet ik nu doen? </t>
   </si>
 </sst>
 </file>
@@ -1434,18 +1434,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C28" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="220" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="255.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="255.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1456,7 +1456,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1467,106 +1467,106 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="C6" s="5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>89</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>85</v>
+        <v>137</v>
       </c>
       <c r="C7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C8" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C9" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C10" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -1643,7 +1643,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1651,21 +1651,21 @@
         <v>27</v>
       </c>
       <c r="C19" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
         <v>34</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C20" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -1676,18 +1676,18 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
         <v>38</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C22" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -1698,18 +1698,18 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>116</v>
+        <v>136</v>
       </c>
       <c r="C24" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -1720,7 +1720,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -1731,18 +1731,18 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
         <v>48</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C27" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
         <v>49</v>
       </c>
@@ -1750,10 +1750,10 @@
         <v>50</v>
       </c>
       <c r="C28" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
         <v>52</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
         <v>53</v>
       </c>
@@ -1772,21 +1772,21 @@
         <v>54</v>
       </c>
       <c r="C30" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
         <v>56</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C31" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
         <v>57</v>
       </c>
@@ -1794,10 +1794,10 @@
         <v>58</v>
       </c>
       <c r="C32" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
         <v>59</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
       <c r="A34" t="s">
         <v>60</v>
       </c>
@@ -1819,84 +1819,84 @@
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
       <c r="A35" t="s">
         <v>62</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
       <c r="A36" t="s">
         <v>63</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C36" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
       <c r="A37" t="s">
         <v>64</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C37" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
       <c r="A38" t="s">
         <v>65</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
       <c r="A39" t="s">
         <v>66</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+    </row>
+    <row r="40" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
       <c r="A40" t="s">
         <v>67</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
       <c r="A41" t="s">
         <v>68</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
       <c r="A42" t="s">
         <v>70</v>
       </c>
@@ -1907,7 +1907,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="58.5" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:3" ht="57.4" x14ac:dyDescent="0.5">
       <c r="A43" t="s">
         <v>72</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
       <c r="A44" t="s">
         <v>74</v>
       </c>
@@ -1926,10 +1926,10 @@
         <v>75</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
       <c r="A45" t="s">
         <v>76</v>
       </c>
@@ -1940,7 +1940,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
       <c r="A46" t="s">
         <v>82</v>
       </c>
@@ -1948,10 +1948,10 @@
         <v>78</v>
       </c>
       <c r="C46" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
       <c r="A47" t="s">
         <v>83</v>
       </c>
@@ -1962,9 +1962,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C48" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1974,6 +1974,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007D896C3867AA3F4EB0C0DE718E7AD517" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="80024e68534539ed8e026f0b5c1f9e6f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c478e2cf-1bd2-4bab-9bac-f508c15c8b21" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3dc892a718835b0a8dea2591f8ec0eaf" ns3:_="">
     <xsd:import namespace="c478e2cf-1bd2-4bab-9bac-f508c15c8b21"/>
@@ -2151,15 +2160,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2167,6 +2167,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EA2A4B5-4A93-4099-B978-EB4B70751D3B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03D7A8B8-DE8F-4F05-BCF1-D0405792B2DC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2180,14 +2188,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EA2A4B5-4A93-4099-B978-EB4B70751D3B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
admin page select inactive users, send messages, message board
</commit_message>
<xml_diff>
--- a/app/static/csv/about_app.xlsx
+++ b/app/static/csv/about_app.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fswleidenunivnl-my.sharepoint.com/personal/a_ghosh_fsw_leidenuniv_nl/Documents/Leiden_CODELAB/Velux_Age/LabSetUp/OnlineTests/Web_based_testing/Online Texts/csvtranslate_v2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\ruchella\agestudy\app\static\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{64033121-2941-41AB-BF0E-307FC7950404}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA987273-4BF7-45BC-98AC-71D5320ECD40}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="about_app" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="139">
   <si>
     <t>tag</t>
   </si>
@@ -308,34 +308,6 @@
   </si>
   <si>
     <t>Ja de app is gratis!</t>
-  </si>
-  <si>
-    <r>
-      <t>Download and open the app</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Download en open de app</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t> </t>
-    </r>
   </si>
   <si>
     <t>You will receive an email from Leiden University within the coming days with further instructions, including your participation ID which needs to be pasted into the App.</t>
@@ -501,9 +473,6 @@
     <t>Android operating system version number as in version 10.0</t>
   </si>
   <si>
-    <t>Rough location as in Leiden, Netherlands (0 decimal position information)</t>
-  </si>
-  <si>
     <t>The timestamp of the touchscreen touch as in 20th Jan 2020, 10h,5m,10s,5ms</t>
   </si>
   <si>
@@ -516,9 +485,6 @@
     <t>Het tijdstempel van de touchscreen-aanraking zoals: 20 januari 2020, 10u, 5m, 10s, 5ms</t>
   </si>
   <si>
-    <t>Ruwe locatie zoals: Leiden, Nederland (informatie over positie met 0 decimalen)</t>
-  </si>
-  <si>
     <t>Versienummer van het Android-besturingssysteem zoals:  versie 10.0</t>
   </si>
   <si>
@@ -541,6 +507,60 @@
   </si>
   <si>
     <t xml:space="preserve">Ik heb me net aangemeld op Agestudy.nl en de app geïnstalleerd, wat moet ik nu doen? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rough location as in Leiden, Netherlands (0 decimal position information, optional) </t>
+  </si>
+  <si>
+    <t>Ruwe locatie zoals: Leiden, Nederland (informatie over positie met 0 decimalen, optioneel)</t>
+  </si>
+  <si>
+    <r>
+      <t>Download and open the app</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF212529"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;a  href="/about_app#data_app"&gt;location&lt;/a&gt; permission is optional)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Download en open de app</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF212529"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(&lt;a  href="/about_app#data_app"&gt;locatietoestemming&lt;/a&gt; is optioneel)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1434,18 +1454,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="220" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="255.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="255.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1456,7 +1476,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1467,7 +1487,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>89</v>
       </c>
@@ -1478,95 +1498,95 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>85</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>86</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>87</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>91</v>
+        <v>137</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C9" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C10" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C11" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1577,7 +1597,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1588,7 +1608,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1599,7 +1619,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1610,7 +1630,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1621,7 +1641,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -1632,7 +1652,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -1643,7 +1663,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1651,21 +1671,21 @@
         <v>27</v>
       </c>
       <c r="C19" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>34</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C20" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -1676,18 +1696,18 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>38</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C22" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -1698,18 +1718,18 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C24" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -1720,7 +1740,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -1731,18 +1751,18 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>48</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C27" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>49</v>
       </c>
@@ -1750,10 +1770,10 @@
         <v>50</v>
       </c>
       <c r="C28" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>52</v>
       </c>
@@ -1764,7 +1784,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>53</v>
       </c>
@@ -1772,21 +1792,21 @@
         <v>54</v>
       </c>
       <c r="C30" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>56</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C31" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>57</v>
       </c>
@@ -1794,10 +1814,10 @@
         <v>58</v>
       </c>
       <c r="C32" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>59</v>
       </c>
@@ -1808,7 +1828,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>60</v>
       </c>
@@ -1819,84 +1839,84 @@
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>62</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>63</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C36" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>64</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C37" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>65</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>66</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
+    </row>
+    <row r="40" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>67</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>68</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>70</v>
       </c>
@@ -1907,7 +1927,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="57.4" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:3" ht="58.5" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>72</v>
       </c>
@@ -1918,7 +1938,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
         <v>74</v>
       </c>
@@ -1926,10 +1946,10 @@
         <v>75</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>76</v>
       </c>
@@ -1940,7 +1960,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>82</v>
       </c>
@@ -1948,10 +1968,10 @@
         <v>78</v>
       </c>
       <c r="C46" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="17.649999999999999" x14ac:dyDescent="0.5">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
         <v>83</v>
       </c>
@@ -1959,13 +1979,11 @@
         <v>79</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C48" t="s">
-        <v>116</v>
-      </c>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+      <c r="B48" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1974,15 +1992,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007D896C3867AA3F4EB0C0DE718E7AD517" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="80024e68534539ed8e026f0b5c1f9e6f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c478e2cf-1bd2-4bab-9bac-f508c15c8b21" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3dc892a718835b0a8dea2591f8ec0eaf" ns3:_="">
     <xsd:import namespace="c478e2cf-1bd2-4bab-9bac-f508c15c8b21"/>
@@ -2160,6 +2169,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2167,14 +2185,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EA2A4B5-4A93-4099-B978-EB4B70751D3B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03D7A8B8-DE8F-4F05-BCF1-D0405792B2DC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2188,6 +2198,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EA2A4B5-4A93-4099-B978-EB4B70751D3B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
EEG transportation cost, reminders subscribe/unsubscribe, query inactive users x weeks and see which users are signed up for reminders, text changes
</commit_message>
<xml_diff>
--- a/app/static/csv/about_app.xlsx
+++ b/app/static/csv/about_app.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\ruchella\agestudy\app\static\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA987273-4BF7-45BC-98AC-71D5320ECD40}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89594F12-FB32-46C8-A74C-6821CE40F2D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="142">
   <si>
     <t>tag</t>
   </si>
@@ -70,25 +70,7 @@
     <t>li3</t>
   </si>
   <si>
-    <t xml:space="preserve">Stap 1. KOPIEER de ID uit de e-mail. </t>
-  </si>
-  <si>
-    <t>Stap 2. Start de app. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stap 3. In ‘participate’ kunt u de ID plakken. Volg de gele vlekken om te plakken. </t>
-  </si>
-  <si>
     <t>Please paste this ID into any Android smartphone tablet that you (alone) use</t>
-  </si>
-  <si>
-    <t>Step 1. COPY the ID from the email.</t>
-  </si>
-  <si>
-    <t>Step 2. Launch the App.</t>
-  </si>
-  <si>
-    <t>Step 3. In ‘participate’, you can paste the ID. Follow the yellow spots to paste.</t>
   </si>
   <si>
     <t>h15</t>
@@ -343,12 +325,6 @@
     <t xml:space="preserve">De eenvoudigste manier is om in het zoekveld van de instellingen ‘Toegang gebruiksgegevens’ te zoeken. Klik daarop en blader naar TapCounter en stel het in. Zie de onderstaande stappen: </t>
   </si>
   <si>
-    <t>Ik heb zojuist een e-mail ontvangen van de Universiteit Leiden met mijn deelname-ID, wat moet ik hiermee doen?</t>
-  </si>
-  <si>
-    <t>I just got an email from Leiden University with my participation ID, what should I do with it?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ik heb zojuist een e-mail ontvangen van de Universiteit Leiden met het verzoek om een ‘handmatige synchronisatie’, hoe kan ik dat doen? </t>
   </si>
   <si>
@@ -365,32 +341,6 @@
   </si>
   <si>
     <t>I just got an email from Leiden University requesting I re-instate the ‘Usage access’ permissions, what do I do?</t>
-  </si>
-  <si>
-    <r>
-      <t>Type “QuantActions TapCounter” in de zoekbalk. &lt;b&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF212529"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Voer het precies zo in.&lt;/b&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF212529"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t> Zorg ervoor dat u de app downloadt van de maker genaamd Quant{Actions} OF klik &lt;a target=_blank_  href="https://play.google.com/store/apps/details?id=com.quantactions.tapcounter"&gt;HIER&lt;/a&gt;</t>
-    </r>
   </si>
   <si>
     <r>
@@ -560,6 +510,66 @@
         <scheme val="minor"/>
       </rPr>
       <t>(&lt;a  href="/about_app#data_app"&gt;locatietoestemming&lt;/a&gt; is optioneel)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">How do I activate the TapCounter App to the study? </t>
+  </si>
+  <si>
+    <t>Hoe activeer ik de Tapcounter App voor het onderzoek?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step 1. Log in and go to the&lt;a href="/account"&gt; account&lt;/a&gt; tab </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Stap 1. Log in en ga naar het &lt;a href="/account"&gt; account &lt;/a&gt; tabblad</t>
+  </si>
+  <si>
+    <t>Stap 4. Richt de camera op de QR-code op de pagina</t>
+  </si>
+  <si>
+    <t>Step 4. Point the camera at the QR code on the page</t>
+  </si>
+  <si>
+    <t>li4</t>
+  </si>
+  <si>
+    <t>Step 3. Open the QR-Code scanner by clicking on</t>
+  </si>
+  <si>
+    <t>Step 2. Open the TapCounter App and press the menu button</t>
+  </si>
+  <si>
+    <t>Stap 2. Open de TapCounter App en druk op de menuknop</t>
+  </si>
+  <si>
+    <t>Stap 3. Open de QR-codescanner door te klikken op</t>
+  </si>
+  <si>
+    <r>
+      <t>Typ “QuantActions TapCounter” in de zoekbalk. &lt;b&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF212529"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Voer het precies zo in.&lt;/b&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF212529"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> Zorg ervoor dat u de app downloadt van de maker genaamd Quant{Actions} OF klik &lt;a target=_blank_  href="https://play.google.com/store/apps/details?id=com.quantactions.tapcounter"&gt;HIER&lt;/a&gt;</t>
     </r>
   </si>
 </sst>
@@ -1086,7 +1096,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1096,6 +1106,9 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1452,10 +1465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1489,46 +1502,46 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C3" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -1536,10 +1549,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="C7" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.4">
@@ -1547,10 +1560,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C8" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -1558,10 +1571,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="C9" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.4">
@@ -1569,10 +1582,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="C10" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -1580,10 +1593,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
       <c r="C11" t="s">
-        <v>98</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.4">
@@ -1591,21 +1604,21 @@
         <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" t="s">
-        <v>16</v>
+        <v>132</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.4">
@@ -1613,377 +1626,388 @@
         <v>14</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>21</v>
+        <v>138</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>15</v>
       </c>
-      <c r="B15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+      <c r="B15" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>24</v>
+        <v>136</v>
+      </c>
+      <c r="B16" t="s">
+        <v>135</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
         <v>25</v>
-      </c>
-      <c r="C17" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" t="s">
         <v>26</v>
-      </c>
-      <c r="C18" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" t="s">
         <v>27</v>
-      </c>
-      <c r="C19" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>101</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>103</v>
+        <v>30</v>
       </c>
       <c r="C22" t="s">
-        <v>102</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>43</v>
+        <v>95</v>
       </c>
       <c r="C23" t="s">
-        <v>39</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>110</v>
+        <v>36</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>132</v>
+        <v>37</v>
       </c>
       <c r="C24" t="s">
-        <v>111</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>101</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>40</v>
+        <v>123</v>
+      </c>
+      <c r="C25" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" t="s">
-        <v>41</v>
+        <v>38</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>104</v>
+        <v>39</v>
       </c>
       <c r="C27" t="s">
-        <v>94</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>50</v>
+        <v>96</v>
       </c>
       <c r="C28" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C29" t="s">
-        <v>55</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C30" t="s">
-        <v>112</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>105</v>
+        <v>48</v>
       </c>
       <c r="C31" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>58</v>
+        <v>97</v>
       </c>
       <c r="C32" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C33" t="s">
-        <v>55</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="C34" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>129</v>
+        <v>55</v>
+      </c>
+      <c r="C35" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C36" t="s">
-        <v>128</v>
+        <v>111</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="C37" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>136</v>
+        <v>113</v>
+      </c>
+      <c r="C38" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="58.5" x14ac:dyDescent="0.4">
+        <v>116</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>65</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="58.5" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>93</v>
+        <v>67</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C46" t="s">
-        <v>113</v>
+        <v>71</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>114</v>
+        <v>72</v>
+      </c>
+      <c r="C47" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="18" x14ac:dyDescent="0.4">
-      <c r="B48" s="2"/>
+      <c r="A48" t="s">
+        <v>77</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" ht="18" x14ac:dyDescent="0.4">
+      <c r="B49" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
text changes, welcome email, eeg page and about app
</commit_message>
<xml_diff>
--- a/app/static/csv/about_app.xlsx
+++ b/app/static/csv/about_app.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\ruchella\agestudy\app\static\csv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\rushkock\agestudyenv\agestudy\app\static\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89594F12-FB32-46C8-A74C-6821CE40F2D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A924629C-431D-41ED-8714-64C7311E1E55}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="about_app" sheetId="1" r:id="rId1"/>
@@ -233,9 +233,6 @@
   </si>
   <si>
     <t>p16</t>
-  </si>
-  <si>
-    <t>For this study, the research team at Leiden University is using this App. This App is operated by the University of Zurich Spin-off QuantActions Ltd (Lausanne, Switzerland) and you can find its detailed privacy policy here. Google PlayStore is used to distribute this App to users like you.</t>
   </si>
   <si>
     <t xml:space="preserve">How do I stop the App from recording data? </t>
@@ -259,9 +256,6 @@
     </r>
   </si>
   <si>
-    <t>Het onderzoeksteam van de Universiteit Leiden gebruikt deze app voor dit onderzoek. Deze app wordt beheerd door de University of Zurich Spin-off QuantActions Ltd (Lausanne, Zwitserland) en u kunt het gedetailleerde privacybeleid hier vinden. Google PlayStore wordt gebruikt om deze app te distribueren naar gebruikers zoals u. </t>
-  </si>
-  <si>
     <t>h24</t>
   </si>
   <si>
@@ -329,9 +323,6 @@
   </si>
   <si>
     <t>I just got an email from Leiden University requesting a ‘manual sync’, how do I do that?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ik heb zojuist een e-mail ontvangen van de Universiteit Leiden met mijn APP-ID, hoe stuur ik het naar u op? </t>
   </si>
   <si>
     <t>I just got an email from Leiden University requesting my APP ID, what is it and how do I send it to you?</t>
@@ -571,6 +562,15 @@
       </rPr>
       <t> Zorg ervoor dat u de app downloadt van de maker genaamd Quant{Actions} OF klik &lt;a target=_blank_  href="https://play.google.com/store/apps/details?id=com.quantactions.tapcounter"&gt;HIER&lt;/a&gt;</t>
     </r>
+  </si>
+  <si>
+    <t>Ik heb zojuist een e-mail ontvangen van de Universiteit Leiden met de vraag om mijn APP-ID toe te sturen, hoe doe ik dat?</t>
+  </si>
+  <si>
+    <t>For this study, the research team at Leiden University is using this App. This App is operated by the University of Zurich Spin-off QuantActions Ltd (Lausanne, Switzerland) and you can find its detailed privacy policy &lt;a target=_blank_  href="https://quantactions.com/privacy/"&gt;here&lt;/a&gt;. Google PlayStore is used to distribute this App to users like you.</t>
+  </si>
+  <si>
+    <t>Het onderzoeksteam van de Universiteit Leiden gebruikt deze app voor dit onderzoek. Deze app wordt beheerd door de University of Zurich Spin-off QuantActions Ltd (Lausanne, Zwitserland) en u kunt het gedetailleerde privacybeleid &lt;a target=_blank_  href="https://quantactions.com/privacy/"&gt;hier&lt;/a&gt; vinden. Google PlayStore wordt gebruikt om deze app te distribueren naar gebruikers zoals u. </t>
   </si>
 </sst>
 </file>
@@ -1467,18 +1467,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="C34" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="220" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="255.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="255.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1500,106 +1500,106 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" t="s">
         <v>82</v>
       </c>
-      <c r="C3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>81</v>
-      </c>
       <c r="B6" s="5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C11" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1610,51 +1610,51 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B16" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C16" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1687,7 +1687,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1695,21 +1695,21 @@
         <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>28</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C21" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -1720,18 +1720,18 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>32</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C23" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -1742,18 +1742,18 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C25" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>40</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -1775,18 +1775,18 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C28" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -1794,10 +1794,10 @@
         <v>44</v>
       </c>
       <c r="C29" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>47</v>
       </c>
@@ -1816,21 +1816,21 @@
         <v>48</v>
       </c>
       <c r="C31" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>50</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C32" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>51</v>
       </c>
@@ -1838,10 +1838,10 @@
         <v>52</v>
       </c>
       <c r="C33" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>53</v>
       </c>
@@ -1852,7 +1852,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>54</v>
       </c>
@@ -1863,84 +1863,84 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>56</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>57</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C37" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>58</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C38" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>59</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>60</v>
       </c>
       <c r="B40" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+    </row>
+    <row r="41" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>61</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>62</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>64</v>
       </c>
@@ -1948,10 +1948,10 @@
         <v>65</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="58.5" x14ac:dyDescent="0.4">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="58.2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>66</v>
       </c>
@@ -1959,10 +1959,10 @@
         <v>67</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>68</v>
       </c>
@@ -1970,43 +1970,43 @@
         <v>69</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="18" x14ac:dyDescent="0.4">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>70</v>
       </c>
       <c r="B46" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>74</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C47" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" ht="18" x14ac:dyDescent="0.4">
-      <c r="A47" t="s">
-        <v>76</v>
-      </c>
-      <c r="B47" s="2" t="s">
+      <c r="B48" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C47" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="18" x14ac:dyDescent="0.4">
-      <c r="A48" t="s">
-        <v>77</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="C48" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2" ht="18" x14ac:dyDescent="0.4">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B49" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
apple phone support added, participation and debriefing letter update
</commit_message>
<xml_diff>
--- a/app/static/csv/about_app.xlsx
+++ b/app/static/csv/about_app.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\rushkock\agestudyenv\agestudy\app\static\csv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\rushkock\agestudy\app\static\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A924629C-431D-41ED-8714-64C7311E1E55}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881A3F19-8565-4F23-BC92-76B270AF6029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="about_app" sheetId="1" r:id="rId1"/>
@@ -334,29 +334,141 @@
     <t>I just got an email from Leiden University requesting I re-instate the ‘Usage access’ permissions, what do I do?</t>
   </si>
   <si>
+    <t>Ga naar de &lt;a target=_blank_  href="https://play.google.com/store/"&gt;Google Play Store&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Go to the &lt;a target=_blank_  href="https://play.google.com/store/"&gt;Google Play Store&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>p8a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Om de APP-ID te sturen, open uw e-mail app (bv. Gmail), maak een nieuw bericht naar agestudy@fsw.leidenuniv.nl en druk met uw vinger op het scherm totdat de ‘Plakken’ optie verschijnt. Als u dan op ‘Plakken’ drukt, zal de APP-ID als tekst verschijnen. </t>
+  </si>
+  <si>
+    <t>De instelling optie ‘Weergeven vóór andere apps’ kan een ander naam hebben in uw telefoon, bijvoorbeeld ‘Bovenaan verschijnen’ of ‘Over andere apps tekenen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hoe kan ik de App stoppen met het meten van mijn gegevens? </t>
+  </si>
+  <si>
+    <t>U kunt de App stoppen door deze gewoon te verwijderen. Let op, stuur ons alstublieft een mail om u formeel terug te trekken uit het onderzoek. Om de App te verwijderen, druk lang op het App-icoon en klik op 'Verwijderen'.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start de App eens in de 2-3 dagen. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ja, dit is normaal dit kan de komende uren zo blijven. Als het langer dan een dag duurt, stuur ons dan een e-mail op agestudy@fsw.leidenuniv.nl </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Na installatie van de app zegt mijn app ‘Initialising’ is dit normaal? </t>
+  </si>
+  <si>
+    <t>After installation, my App says it is ‘Initialising’ is this normal?</t>
+  </si>
+  <si>
+    <t>Yes, this is normal and may remain like this for the next few hours. If it persists for more than a day then please email us at agestudy@fsw.leidenuniv.nl</t>
+  </si>
+  <si>
+    <t>The unique identifier randomly generated by the App as in 138xxxiwhhwhh992ef</t>
+  </si>
+  <si>
+    <t>Manufacturer and model of the smartphone as in SAMSUNG A10</t>
+  </si>
+  <si>
+    <t>Android operating system version number as in version 10.0</t>
+  </si>
+  <si>
+    <t>The timestamp of the touchscreen touch as in 20th Jan 2020, 10h,5m,10s,5ms</t>
+  </si>
+  <si>
+    <t>The label of the App in use as in Facebook or Weather</t>
+  </si>
+  <si>
+    <t>If your phone was used in the portrait or landscape mode</t>
+  </si>
+  <si>
+    <t>Het tijdstempel van de touchscreen-aanraking zoals: 20 januari 2020, 10u, 5m, 10s, 5ms</t>
+  </si>
+  <si>
+    <t>Versienummer van het Android-besturingssysteem zoals:  versie 10.0</t>
+  </si>
+  <si>
+    <t>Fabrikant en model van de smartphone zoals: SAMSUNG A10</t>
+  </si>
+  <si>
+    <t>De unieke identificatie die willekeurig door de app wordt gegenereerd, zoals: 138xxxiwhhwhh992ef</t>
+  </si>
+  <si>
+    <t>Het label van de app die gebruik wordt zoals:  Facebook of Weer</t>
+  </si>
+  <si>
+    <t>Of uw telefoon in de staande of liggende modus werd gebruikt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To send the ID via e-mail, open your e-mail app (e.g. Gmail), create a new email to agestudy@fsw.leidenuniv.nl and press the blank e-mail space with your finger until the ‘Paste’ option appears. When you click on ‘Paste’, the ID should show as text in that space. </t>
+  </si>
+  <si>
+    <t>I just signed up on Agestudy.nl and installed the App, what should I do next?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ik heb me net aangemeld op Agestudy.nl en de app geïnstalleerd, wat moet ik nu doen? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rough location as in Leiden, Netherlands (0 decimal position information, optional) </t>
+  </si>
+  <si>
+    <t>Ruwe locatie zoals: Leiden, Nederland (informatie over positie met 0 decimalen, optioneel)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How do I activate the TapCounter App to the study? </t>
+  </si>
+  <si>
+    <t>Hoe activeer ik de Tapcounter App voor het onderzoek?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step 1. Log in and go to the&lt;a href="/account"&gt; account&lt;/a&gt; tab </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Stap 1. Log in en ga naar het &lt;a href="/account"&gt; account &lt;/a&gt; tabblad</t>
+  </si>
+  <si>
+    <t>Stap 4. Richt de camera op de QR-code op de pagina</t>
+  </si>
+  <si>
+    <t>Step 4. Point the camera at the QR code on the page</t>
+  </si>
+  <si>
+    <t>li4</t>
+  </si>
+  <si>
+    <t>Step 3. Open the QR-Code scanner by clicking on</t>
+  </si>
+  <si>
+    <t>Step 2. Open the TapCounter App and press the menu button</t>
+  </si>
+  <si>
+    <t>Stap 2. Open de TapCounter App en druk op de menuknop</t>
+  </si>
+  <si>
+    <t>Stap 3. Open de QR-codescanner door te klikken op</t>
+  </si>
+  <si>
+    <t>Ik heb zojuist een e-mail ontvangen van de Universiteit Leiden met de vraag om mijn APP-ID toe te sturen, hoe doe ik dat?</t>
+  </si>
+  <si>
+    <t>For this study, the research team at Leiden University is using this App. This App is operated by the University of Zurich Spin-off QuantActions Ltd (Lausanne, Switzerland) and you can find its detailed privacy policy &lt;a target=_blank_  href="https://quantactions.com/privacy/"&gt;here&lt;/a&gt;. Google PlayStore and Apple AppStore are used to distribute this App to users like you.</t>
+  </si>
+  <si>
+    <t>Het onderzoeksteam van de Universiteit Leiden gebruikt deze app voor dit onderzoek. Deze app wordt beheerd door de University of Zurich Spin-off QuantActions Ltd (Lausanne, Zwitserland) en u kunt het gedetailleerde privacybeleid &lt;a target=_blank_  href="https://quantactions.com/privacy/"&gt;hier&lt;/a&gt; vinden. Google Play Store en Apple Play Store wordt gebruikt om deze app te distribueren naar gebruikers zoals u. </t>
+  </si>
+  <si>
+    <t>Typ “QuantActions TapCounter” in de zoekbalk.  Zorg ervoor dat u de app downloadt van de maker genaamd Quant{Actions} OF klik &lt;a target=_blank_  href="https://play.google.com/store/apps/details?id=com.quantactions.tapcounter"&gt;HIER&lt;/a&gt;</t>
+  </si>
+  <si>
     <r>
-      <t>Type “QuantActions TapCounter” in the search bar. &lt;b&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF212529"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Put it exactly like that.&lt;/b&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF212529"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t> Make sure you are downloading the app from the creator called Quant{Actions}</t>
+      <t>Type “QuantActions TapCounter” in the search bar. Make sure you are downloading the app from the creator called Quant{Actions}</t>
     </r>
     <r>
       <rPr>
@@ -369,93 +481,6 @@
     </r>
   </si>
   <si>
-    <t>Ga naar de &lt;a target=_blank_  href="https://play.google.com/store/"&gt;Google Play Store&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>Go to the &lt;a target=_blank_  href="https://play.google.com/store/"&gt;Google Play Store&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>p8a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Om de APP-ID te sturen, open uw e-mail app (bv. Gmail), maak een nieuw bericht naar agestudy@fsw.leidenuniv.nl en druk met uw vinger op het scherm totdat de ‘Plakken’ optie verschijnt. Als u dan op ‘Plakken’ drukt, zal de APP-ID als tekst verschijnen. </t>
-  </si>
-  <si>
-    <t>De instelling optie ‘Weergeven vóór andere apps’ kan een ander naam hebben in uw telefoon, bijvoorbeeld ‘Bovenaan verschijnen’ of ‘Over andere apps tekenen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hoe kan ik de App stoppen met het meten van mijn gegevens? </t>
-  </si>
-  <si>
-    <t>U kunt de App stoppen door deze gewoon te verwijderen. Let op, stuur ons alstublieft een mail om u formeel terug te trekken uit het onderzoek. Om de App te verwijderen, druk lang op het App-icoon en klik op 'Verwijderen'.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Start de App eens in de 2-3 dagen. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ja, dit is normaal dit kan de komende uren zo blijven. Als het langer dan een dag duurt, stuur ons dan een e-mail op agestudy@fsw.leidenuniv.nl </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Na installatie van de app zegt mijn app ‘Initialising’ is dit normaal? </t>
-  </si>
-  <si>
-    <t>After installation, my App says it is ‘Initialising’ is this normal?</t>
-  </si>
-  <si>
-    <t>Yes, this is normal and may remain like this for the next few hours. If it persists for more than a day then please email us at agestudy@fsw.leidenuniv.nl</t>
-  </si>
-  <si>
-    <t>The unique identifier randomly generated by the App as in 138xxxiwhhwhh992ef</t>
-  </si>
-  <si>
-    <t>Manufacturer and model of the smartphone as in SAMSUNG A10</t>
-  </si>
-  <si>
-    <t>Android operating system version number as in version 10.0</t>
-  </si>
-  <si>
-    <t>The timestamp of the touchscreen touch as in 20th Jan 2020, 10h,5m,10s,5ms</t>
-  </si>
-  <si>
-    <t>The label of the App in use as in Facebook or Weather</t>
-  </si>
-  <si>
-    <t>If your phone was used in the portrait or landscape mode</t>
-  </si>
-  <si>
-    <t>Het tijdstempel van de touchscreen-aanraking zoals: 20 januari 2020, 10u, 5m, 10s, 5ms</t>
-  </si>
-  <si>
-    <t>Versienummer van het Android-besturingssysteem zoals:  versie 10.0</t>
-  </si>
-  <si>
-    <t>Fabrikant en model van de smartphone zoals: SAMSUNG A10</t>
-  </si>
-  <si>
-    <t>De unieke identificatie die willekeurig door de app wordt gegenereerd, zoals: 138xxxiwhhwhh992ef</t>
-  </si>
-  <si>
-    <t>Het label van de app die gebruik wordt zoals:  Facebook of Weer</t>
-  </si>
-  <si>
-    <t>Of uw telefoon in de staande of liggende modus werd gebruikt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To send the ID via e-mail, open your e-mail app (e.g. Gmail), create a new email to agestudy@fsw.leidenuniv.nl and press the blank e-mail space with your finger until the ‘Paste’ option appears. When you click on ‘Paste’, the ID should show as text in that space. </t>
-  </si>
-  <si>
-    <t>I just signed up on Agestudy.nl and installed the App, what should I do next?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ik heb me net aangemeld op Agestudy.nl en de app geïnstalleerd, wat moet ik nu doen? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rough location as in Leiden, Netherlands (0 decimal position information, optional) </t>
-  </si>
-  <si>
-    <t>Ruwe locatie zoals: Leiden, Nederland (informatie over positie met 0 decimalen, optioneel)</t>
-  </si>
-  <si>
     <r>
       <t>Download and open the app</t>
     </r>
@@ -466,118 +491,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t> (</t>
+      <t xml:space="preserve">. </t>
     </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF212529"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;a  href="/about_app#data_app"&gt;location&lt;/a&gt; permission is optional)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Download en open de app</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF212529"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(&lt;a  href="/about_app#data_app"&gt;locatietoestemming&lt;/a&gt; is optioneel)</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">How do I activate the TapCounter App to the study? </t>
-  </si>
-  <si>
-    <t>Hoe activeer ik de Tapcounter App voor het onderzoek?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Step 1. Log in and go to the&lt;a href="/account"&gt; account&lt;/a&gt; tab </t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Stap 1. Log in en ga naar het &lt;a href="/account"&gt; account &lt;/a&gt; tabblad</t>
-  </si>
-  <si>
-    <t>Stap 4. Richt de camera op de QR-code op de pagina</t>
-  </si>
-  <si>
-    <t>Step 4. Point the camera at the QR code on the page</t>
-  </si>
-  <si>
-    <t>li4</t>
-  </si>
-  <si>
-    <t>Step 3. Open the QR-Code scanner by clicking on</t>
-  </si>
-  <si>
-    <t>Step 2. Open the TapCounter App and press the menu button</t>
-  </si>
-  <si>
-    <t>Stap 2. Open de TapCounter App en druk op de menuknop</t>
-  </si>
-  <si>
-    <t>Stap 3. Open de QR-codescanner door te klikken op</t>
-  </si>
-  <si>
-    <r>
-      <t>Typ “QuantActions TapCounter” in de zoekbalk. &lt;b&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF212529"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Voer het precies zo in.&lt;/b&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF212529"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t> Zorg ervoor dat u de app downloadt van de maker genaamd Quant{Actions} OF klik &lt;a target=_blank_  href="https://play.google.com/store/apps/details?id=com.quantactions.tapcounter"&gt;HIER&lt;/a&gt;</t>
-    </r>
-  </si>
-  <si>
-    <t>Ik heb zojuist een e-mail ontvangen van de Universiteit Leiden met de vraag om mijn APP-ID toe te sturen, hoe doe ik dat?</t>
-  </si>
-  <si>
-    <t>For this study, the research team at Leiden University is using this App. This App is operated by the University of Zurich Spin-off QuantActions Ltd (Lausanne, Switzerland) and you can find its detailed privacy policy &lt;a target=_blank_  href="https://quantactions.com/privacy/"&gt;here&lt;/a&gt;. Google PlayStore is used to distribute this App to users like you.</t>
-  </si>
-  <si>
-    <t>Het onderzoeksteam van de Universiteit Leiden gebruikt deze app voor dit onderzoek. Deze app wordt beheerd door de University of Zurich Spin-off QuantActions Ltd (Lausanne, Zwitserland) en u kunt het gedetailleerde privacybeleid &lt;a target=_blank_  href="https://quantactions.com/privacy/"&gt;hier&lt;/a&gt; vinden. Google PlayStore wordt gebruikt om deze app te distribueren naar gebruikers zoals u. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Download en open de app. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -740,14 +665,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF212529"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF212529"/>
       <name val="Calibri"/>
@@ -1467,18 +1384,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C34" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="220" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="255.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="255.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1489,7 +1406,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1500,7 +1417,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -1511,51 +1428,51 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>77</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>78</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>95</v>
+        <v>139</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>79</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" t="s">
         <v>121</v>
       </c>
-      <c r="C7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1566,40 +1483,40 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C11" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1610,51 +1527,51 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B16" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C16" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1665,7 +1582,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1676,7 +1593,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1687,7 +1604,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1695,10 +1612,10 @@
         <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -1709,7 +1626,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -1720,7 +1637,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -1728,10 +1645,10 @@
         <v>92</v>
       </c>
       <c r="C23" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -1742,18 +1659,18 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C25" t="s">
         <v>98</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C25" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>40</v>
       </c>
@@ -1764,7 +1681,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -1775,7 +1692,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -1786,7 +1703,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -1797,7 +1714,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -1808,7 +1725,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>47</v>
       </c>
@@ -1816,10 +1733,10 @@
         <v>48</v>
       </c>
       <c r="C31" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>50</v>
       </c>
@@ -1830,7 +1747,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>51</v>
       </c>
@@ -1841,7 +1758,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>53</v>
       </c>
@@ -1852,7 +1769,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>54</v>
       </c>
@@ -1863,84 +1780,84 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>56</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>57</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C37" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>58</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C38" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>59</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="40" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>60</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>61</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>62</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>64</v>
       </c>
@@ -1951,7 +1868,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="58.2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" ht="58.5" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
         <v>66</v>
       </c>
@@ -1962,7 +1879,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>68</v>
       </c>
@@ -1973,18 +1890,18 @@
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>70</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
         <v>74</v>
       </c>
@@ -1992,10 +1909,10 @@
         <v>71</v>
       </c>
       <c r="C47" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
         <v>75</v>
       </c>
@@ -2003,10 +1920,10 @@
         <v>72</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" ht="18" x14ac:dyDescent="0.4">
       <c r="B49" s="2"/>
     </row>
   </sheetData>

</xml_diff>